<commit_message>
Subindo alterações no dicionario de dados e documentação
</commit_message>
<xml_diff>
--- a/Documentação/Dicionario de dados - Agendamento.xlsx
+++ b/Documentação/Dicionario de dados - Agendamento.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danto\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danto\Desktop\DATABASE\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAE5630-7E7F-49A0-9231-87B0C167C511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB414D72-70BE-400D-B43E-D7465D3E24A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{102EC5DA-59AB-45C8-86C9-774FD93ABE7B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="222">
   <si>
     <t>DICIONÁRIO DE DADOS</t>
   </si>
@@ -589,6 +589,124 @@
   </si>
   <si>
     <t>Código de identificação da categoria da tabela CATEGORIAS</t>
+  </si>
+  <si>
+    <t>inserir_agendamento</t>
+  </si>
+  <si>
+    <t>Função para inserir um novo agendamento</t>
+  </si>
+  <si>
+    <t>cliente_id INT,
+prestador_id INT,
+data_agendamento DATE,
+hora_inicio TIME,
+hora_fim TIME,
+assunto TEXT</t>
+  </si>
+  <si>
+    <t>listar_agendamentos_prestador</t>
+  </si>
+  <si>
+    <t>prestador_id_input INT,
+data_agendamento_input_de DATE DEFAULT NULL,
+data_agendamento_input_ate DATE DEFAULT NULL</t>
+  </si>
+  <si>
+    <t>listar_agendamentos_cliente</t>
+  </si>
+  <si>
+    <t>Função para listar os agendamentos do cliente</t>
+  </si>
+  <si>
+    <t>Função para listar os agendamentos do prestador de serviço e pelo intervalo de datas</t>
+  </si>
+  <si>
+    <t>cliente_id_input INT,
+data_agendamento_input_de DATE DEFAULT NULL,
+data_agendamento_input_ate DATE DEFAULT NULL</t>
+  </si>
+  <si>
+    <t>deletar_agendamento</t>
+  </si>
+  <si>
+    <t>Função para deletar um agendamento</t>
+  </si>
+  <si>
+    <t>agendamento_id_input INT</t>
+  </si>
+  <si>
+    <t>listar_agendamento_id</t>
+  </si>
+  <si>
+    <t>Função para listar o agendamento pelo codigo de ID do agendamento</t>
+  </si>
+  <si>
+    <t>alterar_agendamento</t>
+  </si>
+  <si>
+    <t>Função para alterar as informações o agendamento</t>
+  </si>
+  <si>
+    <t>agendamento_id_input INT,
+cliente_id_input INT,
+prestador_id_input INT,
+data_agendamento_input DATE,
+hora_inicio_input TIME,
+hora_fim_input TIME,
+assunto_input TEXT,
+status_input VARCHAR</t>
+  </si>
+  <si>
+    <t>listar_cidade_id</t>
+  </si>
+  <si>
+    <t>Função para listar a cidade pelo ID da cidade</t>
+  </si>
+  <si>
+    <t>listar_cidades_estado_id</t>
+  </si>
+  <si>
+    <t>Função para listar a cidade pelo ID do estado</t>
+  </si>
+  <si>
+    <t>estado_id_input INT</t>
+  </si>
+  <si>
+    <t>cidade_id_input INT</t>
+  </si>
+  <si>
+    <t>listar_cidades_prefixo</t>
+  </si>
+  <si>
+    <t>nome_prefix VARCHAR</t>
+  </si>
+  <si>
+    <t>inserir_cidade</t>
+  </si>
+  <si>
+    <t>Função para inserir uma nova cidade</t>
+  </si>
+  <si>
+    <t>nome VARCHAR, estado_id_input INT</t>
+  </si>
+  <si>
+    <t>deletar_cidade</t>
+  </si>
+  <si>
+    <t>Função para deletar uma cidade</t>
+  </si>
+  <si>
+    <t>alterar_cidade</t>
+  </si>
+  <si>
+    <t>Função para alterar as informações de uma cidade</t>
+  </si>
+  <si>
+    <t>Função para listar as cidades conforme o nome encontrado na tabela de Cidades</t>
+  </si>
+  <si>
+    <t>cidade_id_input INT, novo_nome VARCHAR, novo_estado_id INT</t>
   </si>
 </sst>
 </file>
@@ -886,7 +1004,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -896,7 +1014,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -980,6 +1097,22 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -991,13 +1124,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1080,6 +1206,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1087,15 +1222,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1306,7 +1432,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F8C5F065-2463-47BE-8D31-E978BA6C2487}" name="Tabela1" displayName="Tabela1" ref="A134:C140" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F8C5F065-2463-47BE-8D31-E978BA6C2487}" name="Tabela1" displayName="Tabela1" ref="A134:C140" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A134:C140" xr:uid="{F8C5F065-2463-47BE-8D31-E978BA6C2487}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{AF32FA02-F745-4FB8-A531-0654DDAB8DE5}" name="NOME" dataDxfId="2"/>
@@ -1636,8 +1762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70FF0296-5E37-4545-8B0F-3F5151D565D8}">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1656,13 +1782,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" ht="14.4" thickBot="1">
       <c r="A2" t="s">
@@ -1722,7 +1848,7 @@
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1736,13 +1862,13 @@
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="33" t="s">
         <v>32</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1753,13 +1879,13 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="41" t="s">
         <v>88</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1770,13 +1896,13 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="41" t="s">
         <v>89</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -1787,13 +1913,13 @@
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="33" t="s">
         <v>61</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1804,13 +1930,13 @@
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="41" t="s">
         <v>64</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -1821,13 +1947,13 @@
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="33" t="s">
         <v>35</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1838,13 +1964,13 @@
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="41" t="s">
         <v>66</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -1855,13 +1981,13 @@
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="33" t="s">
         <v>38</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1872,13 +1998,13 @@
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="41" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -1889,30 +2015,30 @@
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="33" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1">
+    <row r="16" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="41" t="s">
         <v>78</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -1923,13 +2049,13 @@
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="33" t="s">
         <v>79</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1940,13 +2066,13 @@
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="41" t="s">
         <v>68</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -1957,13 +2083,13 @@
       <c r="A19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="33" t="s">
         <v>80</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1974,13 +2100,13 @@
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="41" t="s">
         <v>71</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -1991,13 +2117,13 @@
       <c r="A21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="33" t="s">
         <v>95</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -2008,113 +2134,113 @@
       <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="33" t="s">
         <v>94</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1">
+    <row r="23" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="33" t="s">
         <v>125</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1">
+    <row r="24" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1">
       <c r="A24" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="D24" s="34"/>
+      <c r="D24" s="33"/>
       <c r="E24" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1">
-      <c r="A25" s="24" t="s">
+    <row r="25" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1">
+      <c r="A25" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="23" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1">
-      <c r="A26" s="24" t="s">
+    <row r="26" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1">
+      <c r="A26" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1">
-      <c r="A27" s="24" t="s">
+    <row r="27" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1">
+      <c r="A27" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="D27" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1">
-      <c r="A28" s="24" t="s">
+    <row r="28" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1">
+      <c r="A28" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="41" t="s">
         <v>168</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -2122,13 +2248,13 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="14.4" thickBot="1">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="23" t="s">
         <v>165</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="27" t="s">
         <v>18</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -2138,31 +2264,31 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1">
-      <c r="A30" s="24" t="s">
+    <row r="30" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1">
+      <c r="A30" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="27" t="s">
+      <c r="D30" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="E30" s="27" t="s">
+      <c r="E30" s="26" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1">
-      <c r="A31" s="29" t="s">
+    <row r="31" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1">
+      <c r="A31" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="23" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -2172,71 +2298,71 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="6" customFormat="1" ht="28.2" thickBot="1">
-      <c r="A32" s="29" t="s">
+    <row r="32" spans="1:5" s="5" customFormat="1" ht="28.2" thickBot="1">
+      <c r="A32" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="25" t="s">
+      <c r="D32" s="24" t="s">
         <v>173</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1">
-      <c r="A33" s="29" t="s">
+    <row r="33" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1">
+      <c r="A33" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="D33" s="39" t="s">
+      <c r="D33" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="6" customFormat="1">
-      <c r="A34" s="29" t="s">
+    <row r="34" spans="1:5" s="5" customFormat="1">
+      <c r="A34" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="40" t="s">
+      <c r="D34" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="E34" s="27" t="s">
+      <c r="E34" s="26" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.4" thickBot="1">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="41" t="s">
+      <c r="D35" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="28" t="s">
+      <c r="E35" s="27" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2244,13 +2370,13 @@
       <c r="A36" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="34" t="s">
+      <c r="D36" s="33" t="s">
         <v>44</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -2261,13 +2387,13 @@
       <c r="A37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="42" t="s">
+      <c r="D37" s="41" t="s">
         <v>47</v>
       </c>
       <c r="E37" s="2" t="s">
@@ -2278,13 +2404,13 @@
       <c r="A38" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="29" t="s">
+      <c r="C38" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="33" t="s">
         <v>45</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -2295,13 +2421,13 @@
       <c r="A39" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="38" t="s">
+      <c r="B39" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="30" t="s">
+      <c r="C39" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="42" t="s">
+      <c r="D39" s="41" t="s">
         <v>46</v>
       </c>
       <c r="E39" s="2" t="s">
@@ -2309,16 +2435,16 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="28.2" thickBot="1">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="37" t="s">
+      <c r="B40" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="29" t="s">
+      <c r="C40" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="34" t="s">
+      <c r="D40" s="33" t="s">
         <v>50</v>
       </c>
       <c r="E40" s="3" t="s">
@@ -2329,13 +2455,13 @@
       <c r="A41" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="38" t="s">
+      <c r="B41" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="30" t="s">
+      <c r="C41" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="42" t="s">
+      <c r="D41" s="41" t="s">
         <v>53</v>
       </c>
       <c r="E41" s="2" t="s">
@@ -2346,13 +2472,13 @@
       <c r="A42" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="29" t="s">
+      <c r="C42" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D42" s="34" t="s">
+      <c r="D42" s="33" t="s">
         <v>93</v>
       </c>
       <c r="E42" s="3" t="s">
@@ -2363,30 +2489,30 @@
       <c r="A43" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="37" t="s">
+      <c r="B43" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="29" t="s">
+      <c r="C43" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="D43" s="34" t="s">
+      <c r="D43" s="33" t="s">
         <v>92</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1">
+    <row r="44" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1">
       <c r="A44" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B44" s="37" t="s">
+      <c r="B44" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="29" t="s">
+      <c r="C44" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="D44" s="34" t="s">
+      <c r="D44" s="33" t="s">
         <v>127</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -2397,13 +2523,13 @@
       <c r="A45" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="38" t="s">
+      <c r="B45" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C45" s="30" t="s">
+      <c r="C45" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="42" t="s">
+      <c r="D45" s="41" t="s">
         <v>53</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -2414,13 +2540,13 @@
       <c r="A46" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="37" t="s">
+      <c r="B46" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="29" t="s">
+      <c r="C46" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D46" s="34" t="s">
+      <c r="D46" s="33" t="s">
         <v>57</v>
       </c>
       <c r="E46" s="3" t="s">
@@ -2431,13 +2557,13 @@
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="38" t="s">
+      <c r="B47" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="30" t="s">
+      <c r="C47" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="D47" s="42" t="s">
+      <c r="D47" s="41" t="s">
         <v>43</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -2448,13 +2574,13 @@
       <c r="A48" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="37" t="s">
+      <c r="B48" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="29" t="s">
+      <c r="C48" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D48" s="34" t="s">
+      <c r="D48" s="33" t="s">
         <v>55</v>
       </c>
       <c r="E48" s="3" t="s">
@@ -2465,13 +2591,13 @@
       <c r="A49" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="38" t="s">
+      <c r="B49" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="30" t="s">
+      <c r="C49" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D49" s="42" t="s">
+      <c r="D49" s="41" t="s">
         <v>56</v>
       </c>
       <c r="E49" s="2" t="s">
@@ -2482,13 +2608,13 @@
       <c r="A50" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="37" t="s">
+      <c r="B50" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="29" t="s">
+      <c r="C50" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="34" t="s">
+      <c r="D50" s="33" t="s">
         <v>58</v>
       </c>
       <c r="E50" s="3" t="s">
@@ -2499,13 +2625,13 @@
       <c r="A51" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B51" s="38" t="s">
+      <c r="B51" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="C51" s="30" t="s">
+      <c r="C51" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D51" s="42" t="s">
+      <c r="D51" s="41" t="s">
         <v>74</v>
       </c>
       <c r="E51" s="2" t="s">
@@ -2516,13 +2642,13 @@
       <c r="A52" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B52" s="37" t="s">
+      <c r="B52" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="C52" s="29" t="s">
+      <c r="C52" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D52" s="34" t="s">
+      <c r="D52" s="33" t="s">
         <v>38</v>
       </c>
       <c r="E52" s="3" t="s">
@@ -2533,13 +2659,13 @@
       <c r="A53" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="38" t="s">
+      <c r="B53" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="C53" s="30" t="s">
+      <c r="C53" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="D53" s="42" t="s">
+      <c r="D53" s="41" t="s">
         <v>76</v>
       </c>
       <c r="E53" s="2" t="s">
@@ -2550,13 +2676,13 @@
       <c r="A54" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B54" s="37" t="s">
+      <c r="B54" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="C54" s="29" t="s">
+      <c r="C54" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D54" s="34" t="s">
+      <c r="D54" s="33" t="s">
         <v>82</v>
       </c>
       <c r="E54" s="3" t="s">
@@ -2567,13 +2693,13 @@
       <c r="A55" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B55" s="38" t="s">
+      <c r="B55" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="C55" s="30" t="s">
+      <c r="C55" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D55" s="42" t="s">
+      <c r="D55" s="41" t="s">
         <v>83</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -2584,7 +2710,7 @@
       <c r="A56" t="s">
         <v>73</v>
       </c>
-      <c r="B56" s="38" t="s">
+      <c r="B56" s="37" t="s">
         <v>81</v>
       </c>
       <c r="C56" s="4" t="s">
@@ -2601,13 +2727,13 @@
       <c r="A57" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B57" s="38" t="s">
+      <c r="B57" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="C57" s="29" t="s">
+      <c r="C57" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D57" s="34" t="s">
+      <c r="D57" s="33" t="s">
         <v>97</v>
       </c>
       <c r="E57" s="3" t="s">
@@ -2618,13 +2744,13 @@
       <c r="A58" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B58" s="37" t="s">
+      <c r="B58" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="C58" s="29" t="s">
+      <c r="C58" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="D58" s="34" t="s">
+      <c r="D58" s="33" t="s">
         <v>96</v>
       </c>
       <c r="E58" s="3" t="s">
@@ -2632,118 +2758,118 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="5" t="s">
         <v>100</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="E59" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="5" t="s">
         <v>100</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D60" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="E60" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="5" t="s">
         <v>100</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="D61" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="E61" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="5" t="s">
         <v>100</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D62" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E62" s="6" t="s">
+      <c r="E62" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="14.4" thickBot="1">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="5" t="s">
         <v>100</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="D63" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E63" s="6" t="s">
+      <c r="E63" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1">
-      <c r="A64" s="6" t="s">
+    <row r="64" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1">
+      <c r="A64" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C64" s="29" t="s">
+      <c r="C64" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D64" s="34" t="s">
+      <c r="D64" s="33" t="s">
         <v>107</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="6" customFormat="1" ht="14.4" thickBot="1">
-      <c r="A65" s="6" t="s">
+    <row r="65" spans="1:7" s="5" customFormat="1" ht="14.4" thickBot="1">
+      <c r="A65" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C65" s="29" t="s">
+      <c r="C65" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="D65" s="34" t="s">
+      <c r="D65" s="33" t="s">
         <v>108</v>
       </c>
       <c r="E65" s="3" t="s">
@@ -2751,475 +2877,547 @@
       </c>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="45" t="s">
+      <c r="A72" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="B72" s="45"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="19"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="18"/>
+      <c r="B72" s="50"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="17"/>
+      <c r="F72" s="17"/>
+      <c r="G72" s="17"/>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="12" t="s">
+      <c r="A73" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B73" s="13" t="s">
+      <c r="B73" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D73" s="6"/>
+      <c r="D73" s="5"/>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="8" t="s">
+      <c r="A74" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B74" s="13" t="s">
+      <c r="B74" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D74" s="6"/>
+      <c r="D74" s="5"/>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="8" t="s">
+      <c r="A75" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B75" s="13" t="s">
+      <c r="B75" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="D75" s="6"/>
+      <c r="D75" s="5"/>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="8" t="s">
+      <c r="A76" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B76" s="13" t="s">
+      <c r="B76" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="D76" s="6"/>
+      <c r="D76" s="5"/>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="8" t="s">
+      <c r="A77" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B77" s="13" t="s">
+      <c r="B77" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D77" s="6"/>
+      <c r="D77" s="5"/>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="8" t="s">
+      <c r="A78" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B78" s="13" t="s">
+      <c r="B78" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="D78" s="6"/>
+      <c r="D78" s="5"/>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="8"/>
-      <c r="B79" s="10"/>
-      <c r="D79" s="6"/>
+      <c r="A79" s="7"/>
+      <c r="B79" s="9"/>
+      <c r="D79" s="5"/>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="8"/>
-      <c r="B80" s="10"/>
-      <c r="D80" s="6"/>
+      <c r="A80" s="7"/>
+      <c r="B80" s="9"/>
+      <c r="D80" s="5"/>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="8"/>
-      <c r="B81" s="10"/>
-      <c r="D81" s="6"/>
+      <c r="A81" s="7"/>
+      <c r="B81" s="9"/>
+      <c r="D81" s="5"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="8"/>
-      <c r="B82" s="10"/>
-      <c r="D82" s="6"/>
+      <c r="A82" s="7"/>
+      <c r="B82" s="9"/>
+      <c r="D82" s="5"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="8"/>
-      <c r="B83" s="10"/>
-      <c r="D83" s="6"/>
+      <c r="A83" s="7"/>
+      <c r="B83" s="9"/>
+      <c r="D83" s="5"/>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="8"/>
-      <c r="B84" s="10"/>
-      <c r="D84" s="7"/>
+      <c r="A84" s="7"/>
+      <c r="B84" s="9"/>
+      <c r="D84" s="6"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="9"/>
-      <c r="B85" s="11"/>
-      <c r="D85" s="6"/>
+      <c r="A85" s="8"/>
+      <c r="B85" s="10"/>
+      <c r="D85" s="5"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="8"/>
-      <c r="B86" s="10"/>
-      <c r="D86" s="6"/>
+      <c r="A86" s="7"/>
+      <c r="B86" s="9"/>
+      <c r="D86" s="5"/>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="8"/>
-      <c r="B87" s="10"/>
-      <c r="D87" s="6"/>
+      <c r="A87" s="7"/>
+      <c r="B87" s="9"/>
+      <c r="D87" s="5"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="8"/>
-      <c r="B88" s="10"/>
-      <c r="D88" s="6"/>
+      <c r="A88" s="7"/>
+      <c r="B88" s="9"/>
+      <c r="D88" s="5"/>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="8"/>
-      <c r="B89" s="10"/>
-      <c r="D89" s="6"/>
+      <c r="A89" s="7"/>
+      <c r="B89" s="9"/>
+      <c r="D89" s="5"/>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="8"/>
-      <c r="B90" s="10"/>
-      <c r="D90" s="6"/>
+      <c r="A90" s="7"/>
+      <c r="B90" s="9"/>
+      <c r="D90" s="5"/>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="8"/>
-      <c r="B91" s="10"/>
-      <c r="D91" s="6"/>
+      <c r="A91" s="7"/>
+      <c r="B91" s="9"/>
+      <c r="D91" s="5"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="8"/>
-      <c r="B92" s="10"/>
-      <c r="D92" s="6"/>
+      <c r="A92" s="7"/>
+      <c r="B92" s="9"/>
+      <c r="D92" s="5"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="8"/>
-      <c r="B93" s="10"/>
-      <c r="D93" s="6"/>
+      <c r="A93" s="7"/>
+      <c r="B93" s="9"/>
+      <c r="D93" s="5"/>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="8"/>
-      <c r="B94" s="10"/>
-      <c r="D94" s="6"/>
+      <c r="A94" s="7"/>
+      <c r="B94" s="9"/>
+      <c r="D94" s="5"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="8"/>
-      <c r="B95" s="10"/>
-      <c r="D95" s="6"/>
+      <c r="A95" s="7"/>
+      <c r="B95" s="9"/>
+      <c r="D95" s="5"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="8"/>
-      <c r="B96" s="10"/>
-      <c r="D96" s="6"/>
+      <c r="A96" s="7"/>
+      <c r="B96" s="9"/>
+      <c r="D96" s="5"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="8"/>
-      <c r="B97" s="10"/>
-      <c r="D97" s="6"/>
+      <c r="A97" s="7"/>
+      <c r="B97" s="9"/>
+      <c r="D97" s="5"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="8"/>
-      <c r="B98" s="10"/>
-      <c r="D98" s="6"/>
+      <c r="A98" s="7"/>
+      <c r="B98" s="9"/>
+      <c r="D98" s="5"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="14"/>
-      <c r="B99" s="15"/>
-      <c r="D99" s="6"/>
+      <c r="A99" s="13"/>
+      <c r="B99" s="14"/>
+      <c r="D99" s="5"/>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="43" t="s">
+      <c r="A102" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="B102" s="43"/>
-      <c r="C102" s="43"/>
+      <c r="B102" s="48"/>
+      <c r="C102" s="48"/>
     </row>
     <row r="103" spans="1:4">
-      <c r="A103" s="12" t="s">
+      <c r="A103" s="11" t="s">
         <v>84</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C103" s="16" t="s">
+      <c r="C103" s="15" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="8" t="s">
+      <c r="A104" s="7" t="s">
         <v>109</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C104" s="10"/>
+      <c r="C104" s="9"/>
     </row>
     <row r="105" spans="1:4">
-      <c r="A105" s="8" t="s">
+      <c r="A105" s="7" t="s">
         <v>128</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C105" s="10" t="s">
+      <c r="C105" s="9" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="8" t="s">
+      <c r="A106" s="7" t="s">
         <v>131</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C106" s="10" t="s">
+      <c r="C106" s="9" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="107" spans="1:4">
-      <c r="A107" s="8" t="s">
+      <c r="A107" s="7" t="s">
         <v>134</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C107" s="10" t="s">
+      <c r="C107" s="9" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="108" spans="1:4">
-      <c r="A108" s="8" t="s">
+      <c r="A108" s="7" t="s">
         <v>137</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C108" s="10" t="s">
+      <c r="C108" s="9" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="69">
-      <c r="A109" s="23" t="s">
+      <c r="A109" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="B109" s="21" t="s">
+      <c r="B109" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="C109" s="33" t="s">
+      <c r="C109" s="32" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="69">
-      <c r="A110" s="22" t="s">
+      <c r="A110" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="B110" s="20" t="s">
+      <c r="B110" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="C110" s="33" t="s">
+      <c r="C110" s="32" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="82.8">
-      <c r="A111" s="22" t="s">
+      <c r="A111" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="B111" s="21" t="s">
+      <c r="B111" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="C111" s="33" t="s">
+      <c r="C111" s="32" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="82.8">
-      <c r="A112" s="22" t="s">
+      <c r="A112" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="B112" s="20" t="s">
+      <c r="B112" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="C112" s="33" t="s">
+      <c r="C112" s="32" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" s="8" t="s">
+      <c r="A113" s="7" t="s">
         <v>151</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C113" s="10"/>
+      <c r="C113" s="9"/>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="8" t="s">
+      <c r="A114" s="7" t="s">
         <v>153</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C114" s="10"/>
+      <c r="C114" s="9"/>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="8" t="s">
+      <c r="A115" s="7" t="s">
         <v>155</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C115" s="11" t="s">
+      <c r="C115" s="10" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
-      <c r="A116" s="9"/>
-      <c r="B116" s="5"/>
-      <c r="C116" s="10"/>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" s="8"/>
-      <c r="B117" s="4"/>
-      <c r="C117" s="10"/>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="A118" s="8"/>
-      <c r="B118" s="4"/>
-      <c r="C118" s="10"/>
+    <row r="116" spans="1:3" ht="82.8">
+      <c r="A116" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="B116" s="47" t="s">
+        <v>189</v>
+      </c>
+      <c r="C116" s="45" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="69">
+      <c r="A117" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="B117" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="C117" s="45" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="69">
+      <c r="A118" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="B118" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="C118" s="45" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="119" spans="1:3">
-      <c r="A119" s="8"/>
-      <c r="B119" s="4"/>
-      <c r="C119" s="10"/>
+      <c r="A119" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C119" s="9" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" s="8"/>
-      <c r="B120" s="4"/>
-      <c r="C120" s="10"/>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" s="8"/>
-      <c r="B121" s="4"/>
-      <c r="C121" s="10"/>
+      <c r="A120" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C120" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="110.4">
+      <c r="A121" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="B121" s="47" t="s">
+        <v>203</v>
+      </c>
+      <c r="C121" s="45" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="122" spans="1:3">
-      <c r="A122" s="8"/>
-      <c r="B122" s="4"/>
-      <c r="C122" s="10"/>
+      <c r="A122" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C122" s="9" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="123" spans="1:3">
-      <c r="A123" s="8"/>
-      <c r="B123" s="4"/>
-      <c r="C123" s="10"/>
+      <c r="A123" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C123" s="9" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" s="8"/>
-      <c r="B124" s="4"/>
-      <c r="C124" s="10"/>
+      <c r="A124" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C124" s="9" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="8"/>
-      <c r="B125" s="4"/>
-      <c r="C125" s="10"/>
+      <c r="A125" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C125" s="9" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="126" spans="1:3">
-      <c r="A126" s="8"/>
-      <c r="B126" s="4"/>
-      <c r="C126" s="10"/>
-    </row>
-    <row r="127" spans="1:3">
-      <c r="A127" s="8"/>
-      <c r="B127" s="4"/>
-      <c r="C127" s="10"/>
+      <c r="A126" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C126" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="27.6">
+      <c r="A127" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C127" s="45" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="128" spans="1:3">
-      <c r="A128" s="8"/>
+      <c r="A128" s="7"/>
       <c r="B128" s="4"/>
-      <c r="C128" s="10"/>
+      <c r="C128" s="9"/>
     </row>
     <row r="129" spans="1:3">
-      <c r="A129" s="8"/>
+      <c r="A129" s="7"/>
       <c r="B129" s="4"/>
-      <c r="C129" s="10"/>
+      <c r="C129" s="9"/>
     </row>
     <row r="130" spans="1:3">
-      <c r="A130" s="14"/>
-      <c r="B130" s="17"/>
-      <c r="C130" s="15"/>
+      <c r="A130" s="13"/>
+      <c r="B130" s="16"/>
+      <c r="C130" s="14"/>
     </row>
     <row r="133" spans="1:3">
-      <c r="A133" s="46" t="s">
+      <c r="A133" s="51" t="s">
         <v>174</v>
       </c>
-      <c r="B133" s="46"/>
-      <c r="C133" s="46"/>
+      <c r="B133" s="51"/>
+      <c r="C133" s="51"/>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" s="12" t="s">
+      <c r="A134" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B134" s="47" t="s">
+      <c r="B134" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="C134" s="13" t="s">
+      <c r="C134" s="12" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="135" spans="1:3">
-      <c r="A135" s="9" t="s">
+      <c r="A135" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="B135" s="32" t="s">
+      <c r="B135" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C135" s="10" t="s">
+      <c r="C135" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="136" spans="1:3">
-      <c r="A136" s="9" t="s">
+      <c r="A136" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B136" s="32" t="s">
+      <c r="B136" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C136" s="10" t="s">
+      <c r="C136" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="137" spans="1:3">
-      <c r="A137" s="9" t="s">
+      <c r="A137" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B137" s="32" t="s">
+      <c r="B137" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C137" s="10" t="s">
+      <c r="C137" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="138" spans="1:3">
-      <c r="A138" s="9" t="s">
+      <c r="A138" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="B138" s="32" t="s">
+      <c r="B138" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="C138" s="10" t="s">
+      <c r="C138" s="9" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="139" spans="1:3" s="6" customFormat="1">
-      <c r="A139" s="9" t="s">
+    <row r="139" spans="1:3" s="5" customFormat="1">
+      <c r="A139" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="B139" s="32" t="s">
+      <c r="B139" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C139" s="10" t="s">
+      <c r="C139" s="9" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="140" spans="1:3">
-      <c r="A140" s="48" t="s">
+      <c r="A140" s="43" t="s">
         <v>180</v>
       </c>
-      <c r="B140" s="49" t="s">
+      <c r="B140" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C140" s="15" t="s">
+      <c r="C140" s="14" t="s">
         <v>185</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Subindo atualizações nas documentações e nas functions
</commit_message>
<xml_diff>
--- a/Documentação/Dicionario de dados - Agendamento.xlsx
+++ b/Documentação/Dicionario de dados - Agendamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danto\Desktop\DATABASE\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB414D72-70BE-400D-B43E-D7465D3E24A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02816EDE-B58A-4872-BE48-662CE638902D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{102EC5DA-59AB-45C8-86C9-774FD93ABE7B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="240">
   <si>
     <t>DICIONÁRIO DE DADOS</t>
   </si>
@@ -646,6 +646,48 @@
   </si>
   <si>
     <t>Função para alterar as informações o agendamento</t>
+  </si>
+  <si>
+    <t>listar_cidade_id</t>
+  </si>
+  <si>
+    <t>Função para listar a cidade pelo ID da cidade</t>
+  </si>
+  <si>
+    <t>listar_cidades_estado_id</t>
+  </si>
+  <si>
+    <t>Função para listar a cidade pelo ID do estado</t>
+  </si>
+  <si>
+    <t>estado_id_input INT</t>
+  </si>
+  <si>
+    <t>cidade_id_input INT</t>
+  </si>
+  <si>
+    <t>listar_cidades_prefixo</t>
+  </si>
+  <si>
+    <t>inserir_cidade</t>
+  </si>
+  <si>
+    <t>Função para inserir uma nova cidade</t>
+  </si>
+  <si>
+    <t>deletar_cidade</t>
+  </si>
+  <si>
+    <t>Função para deletar uma cidade</t>
+  </si>
+  <si>
+    <t>alterar_cidade</t>
+  </si>
+  <si>
+    <t>Função para alterar as informações de uma cidade</t>
+  </si>
+  <si>
+    <t>Função para listar as cidades conforme o nome encontrado na tabela de Cidades</t>
   </si>
   <si>
     <t>agendamento_id_input INT,
@@ -655,58 +697,76 @@
 hora_inicio_input TIME,
 hora_fim_input TIME,
 assunto_input TEXT,
-status_input VARCHAR</t>
-  </si>
-  <si>
-    <t>listar_cidade_id</t>
-  </si>
-  <si>
-    <t>Função para listar a cidade pelo ID da cidade</t>
-  </si>
-  <si>
-    <t>listar_cidades_estado_id</t>
-  </si>
-  <si>
-    <t>Função para listar a cidade pelo ID do estado</t>
-  </si>
-  <si>
-    <t>estado_id_input INT</t>
-  </si>
-  <si>
-    <t>cidade_id_input INT</t>
-  </si>
-  <si>
-    <t>listar_cidades_prefixo</t>
-  </si>
-  <si>
-    <t>nome_prefix VARCHAR</t>
-  </si>
-  <si>
-    <t>inserir_cidade</t>
-  </si>
-  <si>
-    <t>Função para inserir uma nova cidade</t>
-  </si>
-  <si>
-    <t>nome VARCHAR, estado_id_input INT</t>
-  </si>
-  <si>
-    <t>deletar_cidade</t>
-  </si>
-  <si>
-    <t>Função para deletar uma cidade</t>
-  </si>
-  <si>
-    <t>alterar_cidade</t>
-  </si>
-  <si>
-    <t>Função para alterar as informações de uma cidade</t>
-  </si>
-  <si>
-    <t>Função para listar as cidades conforme o nome encontrado na tabela de Cidades</t>
-  </si>
-  <si>
-    <t>cidade_id_input INT, novo_nome VARCHAR, novo_estado_id INT</t>
+status_input CHAR</t>
+  </si>
+  <si>
+    <t>cidade_id_input INT, novo_nome CHAR, novo_estado_id INT</t>
+  </si>
+  <si>
+    <t>nome CHAR, estado_id_input INT</t>
+  </si>
+  <si>
+    <t>nome_prefix CHAR</t>
+  </si>
+  <si>
+    <t>inserir_ritmo_trabalho</t>
+  </si>
+  <si>
+    <t>Função para adicionar o ritmo de trablho do prestador de serviço na tabela RITMO_TRABALHO</t>
+  </si>
+  <si>
+    <t>prestador_id INT, dia_semana CHAR(20), hora_inicio TIME, hora_fim TIME</t>
+  </si>
+  <si>
+    <t>deletar_ritmo_trabalho</t>
+  </si>
+  <si>
+    <t>Função para deletar o ritmo de trablho do prestador de serviço na tabela RITMO_TRABALHO</t>
+  </si>
+  <si>
+    <t>ritmo_id INT</t>
+  </si>
+  <si>
+    <t>listar_ritmo_trabalho_prestador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Função para listar os ritmos de trabalho do prestador de serviço </t>
+  </si>
+  <si>
+    <t>p_prestador_id INT</t>
+  </si>
+  <si>
+    <t>inserir_excecao</t>
+  </si>
+  <si>
+    <t>Função para adicionar a exceção do prestador de serviço na tabela EXCECOES</t>
+  </si>
+  <si>
+    <t>p_prestador_id INTEGER,
+p_data_bloqueio DATE,
+p_hora_inicio TIME,
+p_hora_fim TIME,
+p_assunto TEXT</t>
+  </si>
+  <si>
+    <t>deletar_excecao</t>
+  </si>
+  <si>
+    <t>Função para deletar a exceção do prestador de serviço na tabela EXCECOES</t>
+  </si>
+  <si>
+    <t>p_id INTEGER</t>
+  </si>
+  <si>
+    <t>p_prestador_id INTEGER,
+p_data_inicio DATE,
+p_data_fim DATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Função para listar as exceções do prestador de serviço </t>
+  </si>
+  <si>
+    <t>listar_excecoes_prestador</t>
   </si>
 </sst>
 </file>
@@ -1420,8 +1480,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7A370113-0EFA-48B9-A0F5-E1CEF21EADA6}" name="Tabela5" displayName="Tabela5" ref="A103:C130" totalsRowShown="0" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="A103:C130" xr:uid="{7A370113-0EFA-48B9-A0F5-E1CEF21EADA6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7A370113-0EFA-48B9-A0F5-E1CEF21EADA6}" name="Tabela5" displayName="Tabela5" ref="A103:C139" totalsRowShown="0" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="A103:C139" xr:uid="{7A370113-0EFA-48B9-A0F5-E1CEF21EADA6}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C99E4950-AD8A-4810-B62C-C3374B1203E3}" name="Nome" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{72F62E16-E319-4FC9-8D03-6FBA1D3469A9}" name="Descrição da Função" dataDxfId="7"/>
@@ -1432,8 +1492,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F8C5F065-2463-47BE-8D31-E978BA6C2487}" name="Tabela1" displayName="Tabela1" ref="A134:C140" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A134:C140" xr:uid="{F8C5F065-2463-47BE-8D31-E978BA6C2487}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F8C5F065-2463-47BE-8D31-E978BA6C2487}" name="Tabela1" displayName="Tabela1" ref="A143:C149" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A143:C149" xr:uid="{F8C5F065-2463-47BE-8D31-E978BA6C2487}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{AF32FA02-F745-4FB8-A531-0654DDAB8DE5}" name="NOME" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{D1839E6E-8E7B-45F6-85D3-C64466048757}" name="TABELA" dataDxfId="1"/>
@@ -1760,10 +1820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70FF0296-5E37-4545-8B0F-3F5151D565D8}">
-  <dimension ref="A1:G140"/>
+  <dimension ref="A1:G149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C126" sqref="C126"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104:C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3253,171 +3313,252 @@
         <v>203</v>
       </c>
       <c r="C121" s="45" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B122" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B122" s="4" t="s">
-        <v>206</v>
-      </c>
       <c r="C122" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B123" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="C123" s="9" t="s">
         <v>208</v>
-      </c>
-      <c r="C123" s="9" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="27.6">
       <c r="A127" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B127" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C127" s="45" t="s">
         <v>219</v>
       </c>
-      <c r="C127" s="45" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
-      <c r="A128" s="7"/>
-      <c r="B128" s="4"/>
-      <c r="C128" s="9"/>
-    </row>
-    <row r="129" spans="1:3">
-      <c r="A129" s="7"/>
-      <c r="B129" s="4"/>
-      <c r="C129" s="9"/>
-    </row>
-    <row r="130" spans="1:3">
-      <c r="A130" s="13"/>
-      <c r="B130" s="16"/>
-      <c r="C130" s="14"/>
-    </row>
-    <row r="133" spans="1:3">
-      <c r="A133" s="51" t="s">
+    </row>
+    <row r="128" spans="1:3" s="5" customFormat="1" ht="27.6">
+      <c r="A128" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C128" s="45" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" s="5" customFormat="1">
+      <c r="A129" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C129" s="45" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" s="5" customFormat="1">
+      <c r="A130" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C130" s="45" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" s="5" customFormat="1" ht="69">
+      <c r="A131" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="B131" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="C131" s="45" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" s="5" customFormat="1">
+      <c r="A132" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C132" s="45" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" s="5" customFormat="1" ht="41.4">
+      <c r="A133" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="B133" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="C133" s="45" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" s="5" customFormat="1">
+      <c r="A134" s="7"/>
+      <c r="B134" s="4"/>
+      <c r="C134" s="45"/>
+    </row>
+    <row r="135" spans="1:3" s="5" customFormat="1">
+      <c r="A135" s="7"/>
+      <c r="B135" s="4"/>
+      <c r="C135" s="45"/>
+    </row>
+    <row r="136" spans="1:3" s="5" customFormat="1">
+      <c r="A136" s="7"/>
+      <c r="B136" s="4"/>
+      <c r="C136" s="45"/>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="7"/>
+      <c r="B137" s="4"/>
+      <c r="C137" s="9"/>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="7"/>
+      <c r="B138" s="4"/>
+      <c r="C138" s="9"/>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="13"/>
+      <c r="B139" s="16"/>
+      <c r="C139" s="14"/>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="51" t="s">
         <v>174</v>
       </c>
-      <c r="B133" s="51"/>
-      <c r="C133" s="51"/>
-    </row>
-    <row r="134" spans="1:3">
-      <c r="A134" s="11" t="s">
+      <c r="B142" s="51"/>
+      <c r="C142" s="51"/>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B134" s="42" t="s">
+      <c r="B143" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="C134" s="12" t="s">
+      <c r="C143" s="12" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
-      <c r="A135" s="8" t="s">
+    <row r="144" spans="1:3">
+      <c r="A144" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="B135" s="31" t="s">
+      <c r="B144" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C135" s="9" t="s">
+      <c r="C144" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
-      <c r="A136" s="8" t="s">
+    <row r="145" spans="1:3">
+      <c r="A145" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B136" s="31" t="s">
+      <c r="B145" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C136" s="9" t="s">
+      <c r="C145" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
-      <c r="A137" s="8" t="s">
+    <row r="146" spans="1:3">
+      <c r="A146" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B137" s="31" t="s">
+      <c r="B146" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C137" s="9" t="s">
+      <c r="C146" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
-      <c r="A138" s="8" t="s">
+    <row r="147" spans="1:3">
+      <c r="A147" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="B138" s="31" t="s">
+      <c r="B147" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="C138" s="9" t="s">
+      <c r="C147" s="9" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="139" spans="1:3" s="5" customFormat="1">
-      <c r="A139" s="8" t="s">
+    <row r="148" spans="1:3" s="5" customFormat="1">
+      <c r="A148" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="B139" s="31" t="s">
+      <c r="B148" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C139" s="9" t="s">
+      <c r="C148" s="9" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
-      <c r="A140" s="43" t="s">
+    <row r="149" spans="1:3">
+      <c r="A149" s="43" t="s">
         <v>180</v>
       </c>
-      <c r="B140" s="44" t="s">
+      <c r="B149" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C140" s="14" t="s">
+      <c r="C149" s="14" t="s">
         <v>185</v>
       </c>
     </row>
@@ -3426,7 +3567,7 @@
     <mergeCell ref="A102:C102"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A133:C133"/>
+    <mergeCell ref="A142:C142"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="40" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>